<commit_message>
added poi for all methods
</commit_message>
<xml_diff>
--- a/poi_test.xlsx
+++ b/poi_test.xlsx
@@ -5,10 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="api" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Data" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="apiKey" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="CoinWithdrawinitiate" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="withdrawID" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="depositID" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="depositNew" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="FiatWithdrawinitiate" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -29,6 +36,69 @@
   </si>
   <si>
     <t xml:space="preserve">LaGTXdtMACLYviUe5Is6AB661Lslnded6BmX7eZD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tesing1.coinsecure@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">satoshis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toAddr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">msg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apikey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1CNugRENyVP6aCbUku6TnryNEs6a41eMKF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h947NqE3snlyWjznSVFW2UaBLRHzIS62CcY1KhjA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">withdrawID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ll1kvbH8C92dwdYlQURF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">depositID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deptype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dena Bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Savings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fiat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">account</t>
   </si>
 </sst>
 </file>
@@ -38,7 +108,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Helvetica Neue"/>
@@ -64,6 +134,20 @@
       <i val="true"/>
       <sz val="10"/>
       <color rgb="FF808080"/>
+      <name val="Helvetica Neue"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica Neue"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
       <family val="0"/>
       <charset val="1"/>
@@ -118,7 +202,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -127,7 +211,19 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -150,30 +246,30 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.4017857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.625"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="9.56696428571429"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.3794642857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.4107142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="7.91517857142857"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="3" t="n">
         <v>8792090543</v>
       </c>
     </row>
@@ -186,4 +282,370 @@
     <oddFooter>&amp;C&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.2767857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.8928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="8.38839285714286"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="tesing1.coinsecure@gmail.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.9330357142857"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2232142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.5133928571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.4553571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.96875"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.26785714285714"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.6160714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.3973214285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50446428571429"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6160714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.9642857142857"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1234</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.875"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.1741071428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.09375"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="51.4196428571429"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>201712345698752</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DataDriven(poi) for all methods
</commit_message>
<xml_diff>
--- a/poi_test.xlsx
+++ b/poi_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="api" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,13 @@
     <sheet name="depositID" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="depositNew" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="FiatWithdrawinitiate" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Info" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="WalletCoinAddrNew" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="WalletCoinNew" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="WalletCoinWithdrawinitiate" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="WalletSendToExchange" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="OrderID" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="AskBidNew" sheetId="15" state="visible" r:id="rId16"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -27,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="36">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -99,6 +106,42 @@
   </si>
   <si>
     <t xml:space="preserve">account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">from</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">offset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">walletID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">walletName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coin Wallet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bDE4PKxaDfblOPc0u6hq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orderID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vol</t>
   </si>
 </sst>
 </file>
@@ -252,9 +295,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.3794642857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.4107142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="7.91517857142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.7901785714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.9375"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="7.44196428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -284,6 +327,333 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5625"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50446428571429"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2232142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.625"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50446428571429"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3169642857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.7276785714286"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.6875"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50446428571429"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>123456</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.7589285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.4821428571429"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.5758928571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8928571428571"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>12345</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.0714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.1517857142857"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -297,9 +667,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.2767857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.8928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="8.38839285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.5669642857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.4196428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="8.15178571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -345,7 +715,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.9330357142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.8705357142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.38839285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -382,14 +753,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2232142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.9642857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.26785714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3571428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.5133928571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.4553571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.96875"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9866071428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.2544642857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8839285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.5714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.2232142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0267857142857"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -450,9 +819,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.6160714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.3973214285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50446428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.3348214285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.26785714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -495,8 +864,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6160714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.9642857142857"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3482142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.78125"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.38839285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -539,7 +909,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.875"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.38839285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.8616071428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.38839285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -594,15 +966,18 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.1741071428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.09375"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="51.4196428571429"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.38839285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.3482142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.8214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.38839285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="50.2008928571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.38839285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -648,4 +1023,63 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.1607142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2276785714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1830357142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.38839285714286"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>1539146092</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>